<commit_message>
Enhance BillingTransaction import functionality by adding 'harga_normal' to required columns and updating the bulk transaction Excel template.
</commit_message>
<xml_diff>
--- a/public/template/bulk_transaction_template_excel.xlsx
+++ b/public/template/bulk_transaction_template_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\febry\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\firman-app\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A4737A-B4E7-479F-8F40-05C61379B170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE4A0D4-B09A-41D8-9FE3-8411E4841693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{36CC24CA-390E-48BD-BBF5-390CC7589B7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36CC24CA-390E-48BD-BBF5-390CC7589B7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>id_pelanggan</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>harga_satuan</t>
+  </si>
+  <si>
+    <t>harga_normal</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5A4597-B490-4785-8EA2-BD4526BCA6B5}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +470,7 @@
     <col min="1" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,50 +489,53 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>